<commit_message>
Added code and results for task 1a and 1b
</commit_message>
<xml_diff>
--- a/Assignment 2/data/gen_data.xlsx
+++ b/Assignment 2/data/gen_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Markus\Dropbox\DTU\46750 - Optimization in Modern Power Systems\Assignment 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marku\Documents\GitHub\46750\Assignment 2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3905384-CFA0-4FD4-8ABE-F6C1C03F5C63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC3382DA-E602-42EC-9DD2-BB1EB5682F8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{F13DEF63-653A-4AAF-8DDB-6130EC382271}"/>
   </bookViews>
@@ -127,32 +127,6 @@
     </r>
     <r>
       <rPr>
-        <i/>
-        <sz val="7"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">− </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>MW</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>R</t>
-    </r>
-    <r>
-      <rPr>
         <sz val="7"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
@@ -204,6 +178,32 @@
   </si>
   <si>
     <t>DT (h)</t>
+  </si>
+  <si>
+    <r>
+      <t>R</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>MW</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -638,7 +638,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,19 +670,19 @@
         <v>4</v>
       </c>
       <c r="F1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="11" t="s">
-        <v>8</v>
-      </c>
       <c r="J1" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>